<commit_message>
Add European Tech Stocks to example data
Extended example_data.xlsx to include 6 European tech stocks alongside
the existing US AI stocks, demonstrating multi-currency (EUR, USD, SEK)
and multi-exchange functionality.

Added stocks:
- ASML (Netherlands) - Semiconductor equipment - 33 shares, 3 purchases
- SAP (Germany) - Enterprise software - 75 shares, 2 purchases
- Infineon (Germany) - Semiconductors - 400 shares, 3 purchases
- Nokia (Finland) - Telecommunications - 900 shares, 2 purchases
- Ericsson (Sweden) - Telecommunications - 1400 shares, 2 purchases
- STMicroelectronics (France) - Semiconductors - 240 shares, 2 purchases

Total transactions increased from 14 to 28.

Updated documentation:
- README.md: Added European Tech Stocks section to example data
- CHANGELOG.md: Documented example data extension in v0.2.0 notes

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,841 +508,1605 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>26-01-2025</t>
+          <t>28-02-2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>11:20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NVIDIA CORP</t>
+          <t>SAP SE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>US67066G1040</t>
+          <t>DE0007164600</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>XET</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G2" t="n">
-        <v>130.11</v>
+        <v>165.8</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2274.32</v>
+        <v>7461</v>
       </c>
       <c r="J2" t="n">
-        <v>2274.86</v>
+        <v>-7461.78</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XETR</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1234567892</t>
-        </is>
+        <v>0.78</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1234567923</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>04-03-2025</t>
+          <t>15-03-2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15:24</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MICROSOFT CORP</t>
+          <t>ASML HOLDING NV</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>US5949181045</t>
+          <t>NL0010273215</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>EAM</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>430.77</v>
+        <v>850.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4359.39</v>
+        <v>12757.5</v>
       </c>
       <c r="J3" t="n">
-        <v>4360.41</v>
+        <v>-12758.32</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XAMS</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>1234567896</t>
-        </is>
+        <v>0.82</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1234567920</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>04-03-2025</t>
+          <t>18-03-2024</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NVIDIA CORP</t>
+          <t>TELEFONAKTIEBOLAGET LM ERICSSON-B</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>US67066G1040</t>
+          <t>SE0000108656</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>TDG</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>39</v>
+        <v>800</v>
       </c>
       <c r="G4" t="n">
-        <v>121.74</v>
+        <v>58.5</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>SEK</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>4368.03</v>
+        <v>4212</v>
       </c>
       <c r="J4" t="n">
-        <v>4369.16</v>
+        <v>-4212.65</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>0.92</v>
+          <t>XSTO</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>11.11</t>
+        </is>
       </c>
       <c r="M4" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>1234567891</t>
-        </is>
+        <v>0.65</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1234567930</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>08-04-2025</t>
+          <t>12-04-2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>19:46</t>
+          <t>09:45</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>META PLATFORMS INC</t>
+          <t>INFINEON TECHNOLOGIES AG</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>US30303M1027</t>
+          <t>DE0006231004</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>XET</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="G5" t="n">
-        <v>558.17</v>
+        <v>35.2</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>10270.33</v>
+        <v>6336</v>
       </c>
       <c r="J5" t="n">
-        <v>10271.4</v>
+        <v>-6336.92</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
+          <t>XETR</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
         <v>0.92</v>
       </c>
-      <c r="M5" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>1234567903</t>
-        </is>
+      <c r="N5" t="n">
+        <v>1234567925</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>22-04-2025</t>
+          <t>25-04-2024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>20:41</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NVIDIA CORP</t>
+          <t>STMICROELECTRONICS NV</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>US67066G1040</t>
+          <t>NL0000226223</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>EPA</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="G6" t="n">
-        <v>130.9</v>
+        <v>42.5</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5900.97</v>
+        <v>5950</v>
       </c>
       <c r="J6" t="n">
-        <v>5901.8</v>
+        <v>-5950.72</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XPAR</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>1234567893</t>
-        </is>
+        <v>0.72</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1234567932</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>26-05-2025</t>
+          <t>05-05-2024</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21:02</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ALPHABET INC-CL A</t>
+          <t>NOKIA OYJ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>US02079K3059</t>
+          <t>FI0009000681</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>34</v>
+        <v>500</v>
       </c>
       <c r="G7" t="n">
-        <v>180.72</v>
+        <v>3.85</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5652.92</v>
+        <v>1925</v>
       </c>
       <c r="J7" t="n">
-        <v>5654.88</v>
+        <v>-1925.54</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XHEL</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>1.96</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>1234567897</t>
-        </is>
+        <v>0.54</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1234567928</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>08-06-2025</t>
+          <t>18-06-2024</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ADVANCED MICRO DEVICES</t>
+          <t>SAP SE</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>US0079031078</t>
+          <t>DE0007164600</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>XET</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G8" t="n">
-        <v>145.99</v>
+        <v>178.45</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2551.91</v>
+        <v>5353.5</v>
       </c>
       <c r="J8" t="n">
-        <v>2552.98</v>
+        <v>-5354.15</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XETR</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>1234567900</t>
-        </is>
+        <v>0.65</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1234567924</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15-07-2025</t>
+          <t>22-07-2024</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ADVANCED MICRO DEVICES</t>
+          <t>ASML HOLDING NV</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>US0079031078</t>
+          <t>NL0010273215</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>EAM</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>122.09</v>
+        <v>920.75</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>5616.14</v>
+        <v>9207.5</v>
       </c>
       <c r="J9" t="n">
-        <v>5617.63</v>
+        <v>-9208.15</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XAMS</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>1234567899</t>
-        </is>
+        <v>0.65</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1234567921</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>23-07-2025</t>
+          <t>15-08-2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ALPHABET INC-CL A</t>
+          <t>STMICROELECTRONICS NV</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>US02079K3059</t>
+          <t>NL0000226223</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>EPA</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="G10" t="n">
-        <v>186.59</v>
+        <v>38.75</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>3948.24</v>
+        <v>3875</v>
       </c>
       <c r="J10" t="n">
-        <v>3949.67</v>
+        <v>-3875.58</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XPAR</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>1234567898</t>
-        </is>
+        <v>0.58</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1234567933</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>29-08-2024</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MICROSOFT CORP</t>
+          <t>INFINEON TECHNOLOGIES AG</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>US5949181045</t>
+          <t>DE0006231004</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>XET</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="G11" t="n">
-        <v>426.46</v>
+        <v>31.85</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>5492.8</v>
+        <v>3822</v>
       </c>
       <c r="J11" t="n">
-        <v>5494.45</v>
+        <v>-3822.67</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XETR</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>1234567895</t>
-        </is>
+        <v>0.67</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1234567926</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>20-09-2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ADVANCED MICRO DEVICES</t>
+          <t>NOKIA OYJ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>US0079031078</t>
+          <t>FI0009000681</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>28</v>
+        <v>400</v>
       </c>
       <c r="G12" t="n">
-        <v>124.88</v>
+        <v>4.12</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>3216.91</v>
+        <v>1648</v>
       </c>
       <c r="J12" t="n">
-        <v>3217.94</v>
+        <v>-1648.48</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XHEL</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>1.03</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>1234567901</t>
-        </is>
+        <v>0.48</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1234567929</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>10-10-2024</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>14:10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MICROSOFT CORP</t>
+          <t>TELEFONAKTIEBOLAGET LM ERICSSON-B</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>US5949181045</t>
+          <t>SE0000108656</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>TDG</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>600</v>
       </c>
       <c r="G13" t="n">
-        <v>442.76</v>
+        <v>62.2</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>SEK</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>2036.7</v>
+        <v>3375</v>
       </c>
       <c r="J13" t="n">
-        <v>2037.44</v>
+        <v>-3375.54</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>0.92</v>
+          <t>XSTO</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>11.05</t>
+        </is>
       </c>
       <c r="M13" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>1234567894</t>
-        </is>
+        <v>0.54</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1234567931</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NVIDIA CORP</t>
+          <t>ASML HOLDING NV</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>US67066G1040</t>
+          <t>NL0010273215</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>EAM</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G14" t="n">
-        <v>124.9</v>
+        <v>795.2</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>2527.98</v>
+        <v>6361.6</v>
       </c>
       <c r="J14" t="n">
-        <v>2528.69</v>
+        <v>-6362.14</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>XNAS</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>0.92</v>
-      </c>
+          <t>XAMS</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
+        <v>0.54</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1234567922</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>15-12-2024</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>INFINEON TECHNOLOGIES AG</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>DE0006231004</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>XET</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>100</v>
+      </c>
+      <c r="G15" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>2950</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-2950.58</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>XETR</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1234567927</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>26-01-2025</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NVIDIA CORP</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>US67066G1040</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>19</v>
+      </c>
+      <c r="G16" t="n">
+        <v>130.11</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>2274.32</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2274.86</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1234567892</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04-03-2025</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>20:47</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NVIDIA CORP</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>US67066G1040</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>39</v>
+      </c>
+      <c r="G17" t="n">
+        <v>121.74</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>4368.03</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4369.16</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1234567891</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04-03-2025</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>15:24</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MICROSOFT CORP</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>US5949181045</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>11</v>
+      </c>
+      <c r="G18" t="n">
+        <v>430.77</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>4359.39</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4360.41</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1234567896</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>08-04-2025</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19:46</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>META PLATFORMS INC</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>US30303M1027</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" t="n">
+        <v>558.17</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>10270.33</v>
+      </c>
+      <c r="J19" t="n">
+        <v>10271.4</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1234567903</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>22-04-2025</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NVIDIA CORP</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>US67066G1040</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>49</v>
+      </c>
+      <c r="G20" t="n">
+        <v>130.9</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>5900.97</v>
+      </c>
+      <c r="J20" t="n">
+        <v>5901.8</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1234567893</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>26-05-2025</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ALPHABET INC-CL A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>US02079K3059</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>34</v>
+      </c>
+      <c r="G21" t="n">
+        <v>180.72</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>5652.92</v>
+      </c>
+      <c r="J21" t="n">
+        <v>5654.88</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1234567897</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08-06-2025</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>15:54</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ADVANCED MICRO DEVICES</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>US0079031078</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>19</v>
+      </c>
+      <c r="G22" t="n">
+        <v>145.99</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>2551.91</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2552.98</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1234567900</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>15-07-2025</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ADVANCED MICRO DEVICES</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>US0079031078</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>50</v>
+      </c>
+      <c r="G23" t="n">
+        <v>122.09</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>5616.14</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5617.63</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1234567899</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23-07-2025</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ALPHABET INC-CL A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>US02079K3059</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>23</v>
+      </c>
+      <c r="G24" t="n">
+        <v>186.59</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>3948.24</v>
+      </c>
+      <c r="J24" t="n">
+        <v>3949.67</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1234567898</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MICROSOFT CORP</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>US5949181045</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>14</v>
+      </c>
+      <c r="G25" t="n">
+        <v>426.46</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>5492.8</v>
+      </c>
+      <c r="J25" t="n">
+        <v>5494.45</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1234567895</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>31-08-2025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ADVANCED MICRO DEVICES</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>US0079031078</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>28</v>
+      </c>
+      <c r="G26" t="n">
+        <v>124.88</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>3216.91</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3217.94</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1234567901</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>08-11-2025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MICROSOFT CORP</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>US5949181045</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" t="n">
+        <v>442.76</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>2036.7</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2037.44</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1234567894</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04-12-2025</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15:01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NVIDIA CORP</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>US67066G1040</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>22</v>
+      </c>
+      <c r="G28" t="n">
+        <v>124.9</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>2527.98</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2528.69</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>XNAS</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>20-12-2025</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>17:44</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>META PLATFORMS INC</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>US30303M1027</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>NASDAQ</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="F29" t="n">
         <v>48</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G29" t="n">
         <v>582.4</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="I15" t="n">
+      <c r="I29" t="n">
         <v>25718.78</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J29" t="n">
         <v>25720.19</v>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>XNAS</t>
         </is>
       </c>
-      <c r="L15" t="n">
+      <c r="L29" t="n">
         <v>0.92</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M29" t="n">
         <v>1.41</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>1234567902</t>
-        </is>
+      <c r="N29" t="n">
+        <v>1234567902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>